<commit_message>
Store-, load- and apply button mappings
</commit_message>
<xml_diff>
--- a/docs/Memory.xlsx
+++ b/docs/Memory.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
   <si>
     <t>44</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>version</t>
+  </si>
+  <si>
+    <t>button_mapping_t (Position 1)</t>
+  </si>
+  <si>
+    <t>button_mapping_t (Position 0)</t>
+  </si>
+  <si>
+    <t>button_mapping_t (Position 2)</t>
+  </si>
+  <si>
+    <t>button_mapping_t (Position 3)</t>
   </si>
 </sst>
 </file>
@@ -315,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -375,11 +387,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -408,6 +500,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,7 +832,7 @@
   <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +965,12 @@
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="1"/>
       <c r="G7" s="9" t="s">
         <v>15</v>
@@ -863,10 +984,10 @@
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="1"/>
       <c r="G8" s="9" t="s">
         <v>16</v>
@@ -880,10 +1001,10 @@
       <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="1"/>
       <c r="G9" s="9" t="s">
         <v>17</v>
@@ -897,10 +1018,10 @@
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="1"/>
       <c r="G10" s="9" t="s">
         <v>18</v>
@@ -914,10 +1035,12 @@
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="1"/>
       <c r="G11" s="9" t="s">
         <v>19</v>
@@ -931,10 +1054,10 @@
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="1"/>
       <c r="G12" s="9" t="s">
         <v>20</v>
@@ -948,10 +1071,10 @@
       <c r="A13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="1"/>
       <c r="G13" s="9" t="s">
         <v>21</v>
@@ -965,10 +1088,10 @@
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1"/>
       <c r="G14" s="9" t="s">
         <v>22</v>
@@ -982,10 +1105,12 @@
       <c r="A15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="1"/>
       <c r="G15" s="9" t="s">
         <v>23</v>
@@ -999,10 +1124,10 @@
       <c r="A16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="1"/>
       <c r="G16" s="9" t="s">
         <v>24</v>
@@ -1016,10 +1141,10 @@
       <c r="A17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
         <v>25</v>
@@ -1033,10 +1158,10 @@
       <c r="A18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1"/>
       <c r="G18" s="9" t="s">
         <v>26</v>
@@ -1050,10 +1175,12 @@
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="B19" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="1"/>
       <c r="G19" s="9" t="s">
         <v>27</v>
@@ -1067,10 +1194,10 @@
       <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="1"/>
       <c r="G20" s="9" t="s">
         <v>0</v>
@@ -1084,10 +1211,10 @@
       <c r="A21" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="1"/>
       <c r="G21" s="9" t="s">
         <v>1</v>
@@ -1101,10 +1228,10 @@
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1"/>
       <c r="G22" s="9" t="s">
         <v>2</v>
@@ -1863,8 +1990,12 @@
       <c r="K66" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E10"/>
+    <mergeCell ref="B11:E14"/>
+    <mergeCell ref="B15:E18"/>
+    <mergeCell ref="B19:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>